<commit_message>
marc final diary update 3.17
</commit_message>
<xml_diff>
--- a/diaries/diary-marc-andrada.xlsx
+++ b/diaries/diary-marc-andrada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Marc/Desktop/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10433490-4343-194E-B8F2-F5532D215E3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC30FB3-2934-1848-98E9-2943F9A5E6EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="500" windowWidth="25600" windowHeight="14200" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="145">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -78,24 +78,6 @@
     <t>&lt;01/15/2020&gt;</t>
   </si>
   <si>
-    <t>&lt;6:04&gt;</t>
-  </si>
-  <si>
-    <t>Was able to install everything and write my first entry!</t>
-  </si>
-  <si>
-    <t>Setting up environment, repositories, writing my first diary</t>
-  </si>
-  <si>
-    <t>Me, myself, and I</t>
-  </si>
-  <si>
-    <t>Happy to have figured it out!</t>
-  </si>
-  <si>
-    <t>&lt;12:24&gt;</t>
-  </si>
-  <si>
     <t>&lt;My team and I&gt;</t>
   </si>
   <si>
@@ -396,18 +378,12 @@
     <t>&lt;3/16/2020&gt;</t>
   </si>
   <si>
-    <t>&lt;Wrote our report on our current issue and trying to get a PR approved. Split our report into three sections per Andre and Kaj's requests&gt;</t>
-  </si>
-  <si>
     <t>&lt;Finding a more complex issue is well, complex. Our first issue was fixing annotations so we needed to step up our contributions. We ultimately found something, which although was still a small fix, could potentially be meaningful to the overall system. The PR process is a bit complex as well because Glide requires us to consent to their continuous integration testing, etc before we can officially send a PR. Overall a good learning experience as a whole.&gt;</t>
   </si>
   <si>
     <t>&lt;happy, a bit lonley because of all the isolation due to COVID 19, but the internet is awesome for making friends/talking to people!&gt;</t>
   </si>
   <si>
-    <t>&lt;8:00&gt;</t>
-  </si>
-  <si>
     <t>&lt;Final Reflection&gt;</t>
   </si>
   <si>
@@ -418,6 +394,78 @@
   </si>
   <si>
     <t>&lt;sad the course is over, happy it is spring break, excited to keep learning in this program with my cohort!&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Was able to install everything and write my first entry!&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Setting up environment, repositories, writing my first diary&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Me, myself, and I&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Happy to have figured it out!&gt;</t>
+  </si>
+  <si>
+    <t>&lt;3/17/2020&gt;</t>
+  </si>
+  <si>
+    <t>&lt;10:00&gt;</t>
+  </si>
+  <si>
+    <t>&lt;10:00-4:00&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Worked on our current issue, a solution to it, and trying to get a PR in.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;6:00&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Split our report into three sections per Andre and Kaj's requests, cleaned up other parts of assignment to make it look better.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;When we first started our assignments we were just throwing the questions and answers onto a document without thought to making a nice layout. We have come a long way from that, making our reports look more organized and presentable. It's crazy how something as small as this can be so important to how our overall report is received in the end&gt;</t>
+  </si>
+  <si>
+    <t>&lt;happy to be finished with hw 6!&gt;</t>
+  </si>
+  <si>
+    <t>&lt;3/15/2020&gt;</t>
+  </si>
+  <si>
+    <t>&lt;01/09/2020&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Had our first lecture, talked about using GitHub, making teams, and writing in these diaries.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Excited to learn more about reverse engineering along with some new skills and best practices in the industry.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Excited for the new quarter&gt;</t>
+  </si>
+  <si>
+    <t>&lt;01/16/2020&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Learned some basic strategies for trying to understand systems. Worked on a practical assignment with JPacman. Had a guest speaker from Google!&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Fun lecture, starting to learn some important things I need to take with me into the work field. I liked the part lecture part practical aspect of this course. The guest speaker was very interesting and inspiring because he came from our school and has worked at Google for 20+ years! I hope I can work for and contribute to  awesome companies like that one day.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Happy, a bit tired and hungry because these classes go kind of late :c&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Talked about mental models and some ways to externally model systems (UML). Had a guest speaker as well.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;It was interesting learning these concepts, which are supposedly "common sense" in the work industry, but it allows us to now describe our process. For example mental models is something we inherently do, but now we can verbalize this when we explain how we got to certain conclusions etc. Guest speaker was awesome as well!&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Happy, hungry (always), sleepy-ish&gt;</t>
   </si>
 </sst>
 </file>
@@ -899,10 +947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1019,556 +1067,612 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B11" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="D13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="G10" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+    <row r="14" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="9" t="s">
+      <c r="B15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="B16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+    <row r="17" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="C17" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="136" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="9" t="s">
+      <c r="F17" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="G17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>55</v>
-      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="F23" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="G23" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="10" t="s">
+    </row>
+    <row r="24" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
+      <c r="B24" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="10" t="s">
+      <c r="F24" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="G24" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="B25" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="E25" s="9" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
+      <c r="F25" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="9" t="s">
+      <c r="G25" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="9" t="s">
+    </row>
+    <row r="26" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G21" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="119" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
+      <c r="B26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="F26" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" s="9" t="s">
+      <c r="E27" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
+      <c r="C28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="170" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
+      <c r="E28" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="F28" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="G28" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E24" s="9" t="s">
+    </row>
+    <row r="29" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="B29" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="F29" s="9" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="204" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="9" t="s">
+      <c r="G29" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="B30" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="E30" s="9" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="136" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
+      <c r="F30" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="9" t="s">
+      <c r="G30" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F26" s="9" t="s">
+    </row>
+    <row r="31" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="G26" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="119" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="9" t="s">
+      <c r="B31" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="C31" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="F31" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G31" s="10" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="136" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="272" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="238" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="221" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="272" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="238" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="221" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="272" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G36" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="B32" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="10"/>
-    </row>
-    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="10"/>
-    </row>
-    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="10"/>
     </row>
     <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="9"/>
@@ -2370,6 +2474,33 @@
       <c r="E125" s="9"/>
       <c r="F125" s="9"/>
       <c r="G125" s="10"/>
+    </row>
+    <row r="126" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A126" s="9"/>
+      <c r="B126" s="9"/>
+      <c r="C126" s="9"/>
+      <c r="D126" s="9"/>
+      <c r="E126" s="9"/>
+      <c r="F126" s="9"/>
+      <c r="G126" s="10"/>
+    </row>
+    <row r="127" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A127" s="9"/>
+      <c r="B127" s="9"/>
+      <c r="C127" s="9"/>
+      <c r="D127" s="9"/>
+      <c r="E127" s="9"/>
+      <c r="F127" s="9"/>
+      <c r="G127" s="10"/>
+    </row>
+    <row r="128" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A128" s="9"/>
+      <c r="B128" s="9"/>
+      <c r="C128" s="9"/>
+      <c r="D128" s="9"/>
+      <c r="E128" s="9"/>
+      <c r="F128" s="9"/>
+      <c r="G128" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>